<commit_message>
se implementa el balanceo por python con la lectura de codigos, se agrega la repetitibilidad de lectura de cajas sin duplicar estadisticas
</commit_message>
<xml_diff>
--- a/DataBases/APrueba Bodega.xlsx
+++ b/DataBases/APrueba Bodega.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\EliteFlowerDeploy_V3\DataBases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D80B376-A2E8-4D98-95EB-4FB3C7C4D142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753A5191-A490-450D-844F-D7BE08438ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5109" uniqueCount="1593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5047" uniqueCount="1592">
   <si>
     <t>COMPANY ID</t>
   </si>
@@ -4803,9 +4803,6 @@
   </si>
   <si>
     <t>I LOVE YOU</t>
-  </si>
-  <si>
-    <t>una</t>
   </si>
   <si>
     <t>VASE_ID</t>
@@ -5295,8 +5292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C36539B9-9471-4585-8EAC-B9EBB1AE43E1}">
   <dimension ref="A1:AI4021"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5334,13 +5331,13 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="J1" t="s">
         <v>6</v>
@@ -5355,7 +5352,7 @@
         <v>9</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="O1" t="s">
         <v>10</v>
@@ -5443,9 +5440,6 @@
       <c r="G2" t="s">
         <v>1186</v>
       </c>
-      <c r="H2" t="s">
-        <v>1589</v>
-      </c>
       <c r="I2" t="s">
         <v>114</v>
       </c>
@@ -5547,9 +5541,6 @@
       <c r="G3" t="s">
         <v>1186</v>
       </c>
-      <c r="H3" t="s">
-        <v>1589</v>
-      </c>
       <c r="I3" t="s">
         <v>122</v>
       </c>
@@ -5651,9 +5642,6 @@
       <c r="G4" t="s">
         <v>1186</v>
       </c>
-      <c r="H4" t="s">
-        <v>1589</v>
-      </c>
       <c r="I4" t="s">
         <v>122</v>
       </c>
@@ -5963,9 +5951,6 @@
       <c r="G7" t="s">
         <v>1186</v>
       </c>
-      <c r="H7" t="s">
-        <v>1589</v>
-      </c>
       <c r="I7" t="s">
         <v>114</v>
       </c>
@@ -6067,9 +6052,6 @@
       <c r="G8" t="s">
         <v>1186</v>
       </c>
-      <c r="H8" t="s">
-        <v>1589</v>
-      </c>
       <c r="I8" t="s">
         <v>122</v>
       </c>
@@ -6171,9 +6153,6 @@
       <c r="G9" t="s">
         <v>1186</v>
       </c>
-      <c r="H9" t="s">
-        <v>1589</v>
-      </c>
       <c r="I9" t="s">
         <v>122</v>
       </c>
@@ -6275,9 +6254,6 @@
       <c r="G10" t="s">
         <v>1186</v>
       </c>
-      <c r="H10" t="s">
-        <v>1589</v>
-      </c>
       <c r="I10" t="s">
         <v>114</v>
       </c>
@@ -6379,9 +6355,6 @@
       <c r="G11" t="s">
         <v>1186</v>
       </c>
-      <c r="H11" t="s">
-        <v>1589</v>
-      </c>
       <c r="I11" t="s">
         <v>122</v>
       </c>
@@ -8976,9 +8949,6 @@
       <c r="G36" t="s">
         <v>1186</v>
       </c>
-      <c r="H36" t="s">
-        <v>1589</v>
-      </c>
       <c r="I36" t="s">
         <v>122</v>
       </c>
@@ -9080,9 +9050,6 @@
       <c r="G37" t="s">
         <v>1186</v>
       </c>
-      <c r="H37" t="s">
-        <v>1589</v>
-      </c>
       <c r="I37" t="s">
         <v>114</v>
       </c>
@@ -9184,9 +9151,6 @@
       <c r="G38" t="s">
         <v>1186</v>
       </c>
-      <c r="H38" t="s">
-        <v>1589</v>
-      </c>
       <c r="I38" t="s">
         <v>122</v>
       </c>
@@ -9288,9 +9252,6 @@
       <c r="G39" t="s">
         <v>1186</v>
       </c>
-      <c r="H39" t="s">
-        <v>1589</v>
-      </c>
       <c r="I39" t="s">
         <v>122</v>
       </c>
@@ -9392,9 +9353,6 @@
       <c r="G40" t="s">
         <v>1186</v>
       </c>
-      <c r="H40" t="s">
-        <v>1589</v>
-      </c>
       <c r="I40" t="s">
         <v>122</v>
       </c>
@@ -9600,9 +9558,6 @@
       <c r="G42" t="s">
         <v>1186</v>
       </c>
-      <c r="H42" t="s">
-        <v>1589</v>
-      </c>
       <c r="I42" t="s">
         <v>122</v>
       </c>
@@ -10420,9 +10375,6 @@
       <c r="F50" t="s">
         <v>917</v>
       </c>
-      <c r="G50" t="s">
-        <v>1186</v>
-      </c>
       <c r="H50" t="s">
         <v>85</v>
       </c>
@@ -10524,9 +10476,6 @@
       <c r="F51" t="s">
         <v>969</v>
       </c>
-      <c r="G51" t="s">
-        <v>1186</v>
-      </c>
       <c r="H51" t="s">
         <v>85</v>
       </c>
@@ -10628,9 +10577,6 @@
       <c r="F52" t="s">
         <v>1121</v>
       </c>
-      <c r="G52" t="s">
-        <v>1186</v>
-      </c>
       <c r="H52" t="s">
         <v>85</v>
       </c>
@@ -10732,9 +10678,6 @@
       <c r="F53" t="s">
         <v>382</v>
       </c>
-      <c r="G53" t="s">
-        <v>1186</v>
-      </c>
       <c r="H53" t="s">
         <v>85</v>
       </c>
@@ -10836,9 +10779,6 @@
       <c r="F54" t="s">
         <v>382</v>
       </c>
-      <c r="G54" t="s">
-        <v>1186</v>
-      </c>
       <c r="I54" t="s">
         <v>114</v>
       </c>
@@ -10937,9 +10877,6 @@
       <c r="F55" t="s">
         <v>186</v>
       </c>
-      <c r="G55" t="s">
-        <v>1186</v>
-      </c>
       <c r="H55" t="s">
         <v>85</v>
       </c>
@@ -11041,12 +10978,6 @@
       <c r="F56" t="s">
         <v>382</v>
       </c>
-      <c r="G56" t="s">
-        <v>1186</v>
-      </c>
-      <c r="H56" t="s">
-        <v>1589</v>
-      </c>
       <c r="I56" t="s">
         <v>114</v>
       </c>
@@ -11145,12 +11076,6 @@
       <c r="F57" t="s">
         <v>33</v>
       </c>
-      <c r="G57" t="s">
-        <v>1186</v>
-      </c>
-      <c r="H57" t="s">
-        <v>1589</v>
-      </c>
       <c r="I57" t="s">
         <v>114</v>
       </c>
@@ -11249,12 +11174,6 @@
       <c r="F58" t="s">
         <v>382</v>
       </c>
-      <c r="G58" t="s">
-        <v>1186</v>
-      </c>
-      <c r="H58" t="s">
-        <v>1589</v>
-      </c>
       <c r="I58" t="s">
         <v>94</v>
       </c>
@@ -11353,12 +11272,6 @@
       <c r="F59" t="s">
         <v>382</v>
       </c>
-      <c r="G59" t="s">
-        <v>1186</v>
-      </c>
-      <c r="H59" t="s">
-        <v>1589</v>
-      </c>
       <c r="I59" t="s">
         <v>122</v>
       </c>
@@ -11457,12 +11370,6 @@
       <c r="F60" t="s">
         <v>825</v>
       </c>
-      <c r="G60" t="s">
-        <v>1186</v>
-      </c>
-      <c r="H60" t="s">
-        <v>1589</v>
-      </c>
       <c r="I60" t="s">
         <v>114</v>
       </c>
@@ -11561,12 +11468,6 @@
       <c r="F61" t="s">
         <v>382</v>
       </c>
-      <c r="G61" t="s">
-        <v>1186</v>
-      </c>
-      <c r="H61" t="s">
-        <v>1589</v>
-      </c>
       <c r="I61" t="s">
         <v>122</v>
       </c>
@@ -11665,12 +11566,6 @@
       <c r="F62" t="s">
         <v>382</v>
       </c>
-      <c r="G62" t="s">
-        <v>1186</v>
-      </c>
-      <c r="H62" t="s">
-        <v>1589</v>
-      </c>
       <c r="I62" t="s">
         <v>122</v>
       </c>
@@ -11769,12 +11664,6 @@
       <c r="F63" t="s">
         <v>382</v>
       </c>
-      <c r="G63" t="s">
-        <v>1186</v>
-      </c>
-      <c r="H63" t="s">
-        <v>1589</v>
-      </c>
       <c r="I63" t="s">
         <v>122</v>
       </c>
@@ -11873,9 +11762,6 @@
       <c r="F64" t="s">
         <v>1074</v>
       </c>
-      <c r="G64" t="s">
-        <v>1186</v>
-      </c>
       <c r="I64" t="s">
         <v>114</v>
       </c>
@@ -11974,9 +11860,6 @@
       <c r="F65" t="s">
         <v>969</v>
       </c>
-      <c r="G65" t="s">
-        <v>1186</v>
-      </c>
       <c r="I65" t="s">
         <v>114</v>
       </c>
@@ -12075,9 +11958,6 @@
       <c r="F66" t="s">
         <v>382</v>
       </c>
-      <c r="G66" t="s">
-        <v>1186</v>
-      </c>
       <c r="I66" t="s">
         <v>114</v>
       </c>
@@ -12176,9 +12056,6 @@
       <c r="F67" t="s">
         <v>1074</v>
       </c>
-      <c r="G67" t="s">
-        <v>1186</v>
-      </c>
       <c r="H67" t="s">
         <v>85</v>
       </c>
@@ -12283,9 +12160,6 @@
       <c r="G68" t="s">
         <v>1186</v>
       </c>
-      <c r="H68" t="s">
-        <v>1589</v>
-      </c>
       <c r="I68" t="s">
         <v>122</v>
       </c>
@@ -12387,9 +12261,6 @@
       <c r="G69" t="s">
         <v>1188</v>
       </c>
-      <c r="H69" t="s">
-        <v>1589</v>
-      </c>
       <c r="I69" t="s">
         <v>114</v>
       </c>
@@ -12491,9 +12362,6 @@
       <c r="G70" t="s">
         <v>1188</v>
       </c>
-      <c r="H70" t="s">
-        <v>1589</v>
-      </c>
       <c r="I70" t="s">
         <v>114</v>
       </c>
@@ -12595,9 +12463,6 @@
       <c r="G71" t="s">
         <v>1188</v>
       </c>
-      <c r="H71" t="s">
-        <v>1589</v>
-      </c>
       <c r="I71" t="s">
         <v>122</v>
       </c>
@@ -14039,9 +13904,6 @@
       <c r="G85" t="s">
         <v>1188</v>
       </c>
-      <c r="H85" t="s">
-        <v>1589</v>
-      </c>
       <c r="I85" t="s">
         <v>122</v>
       </c>
@@ -14143,9 +14005,6 @@
       <c r="G86" t="s">
         <v>1188</v>
       </c>
-      <c r="H86" t="s">
-        <v>1589</v>
-      </c>
       <c r="I86" t="s">
         <v>94</v>
       </c>
@@ -14247,9 +14106,6 @@
       <c r="G87" t="s">
         <v>1188</v>
       </c>
-      <c r="H87" t="s">
-        <v>1589</v>
-      </c>
       <c r="I87" t="s">
         <v>114</v>
       </c>
@@ -14351,9 +14207,6 @@
       <c r="G88" t="s">
         <v>1188</v>
       </c>
-      <c r="H88" t="s">
-        <v>1589</v>
-      </c>
       <c r="I88" t="s">
         <v>122</v>
       </c>
@@ -14764,9 +14617,6 @@
       <c r="G92" t="s">
         <v>1188</v>
       </c>
-      <c r="H92" t="s">
-        <v>1589</v>
-      </c>
       <c r="I92" t="s">
         <v>122</v>
       </c>
@@ -14868,9 +14718,6 @@
       <c r="G93" t="s">
         <v>1188</v>
       </c>
-      <c r="H93" t="s">
-        <v>1589</v>
-      </c>
       <c r="I93" t="s">
         <v>94</v>
       </c>
@@ -14972,9 +14819,6 @@
       <c r="G94" t="s">
         <v>1188</v>
       </c>
-      <c r="H94" t="s">
-        <v>1589</v>
-      </c>
       <c r="I94" t="s">
         <v>122</v>
       </c>
@@ -15076,9 +14920,6 @@
       <c r="G95" t="s">
         <v>1188</v>
       </c>
-      <c r="H95" t="s">
-        <v>1589</v>
-      </c>
       <c r="I95" t="s">
         <v>122</v>
       </c>
@@ -15180,9 +15021,6 @@
       <c r="G96" t="s">
         <v>1188</v>
       </c>
-      <c r="H96" t="s">
-        <v>1589</v>
-      </c>
       <c r="I96" t="s">
         <v>122</v>
       </c>
@@ -15284,9 +15122,6 @@
       <c r="G97" t="s">
         <v>1188</v>
       </c>
-      <c r="H97" t="s">
-        <v>1589</v>
-      </c>
       <c r="I97" t="s">
         <v>94</v>
       </c>
@@ -16425,9 +16260,6 @@
       <c r="G108" t="s">
         <v>1187</v>
       </c>
-      <c r="H108" t="s">
-        <v>1589</v>
-      </c>
       <c r="I108" t="s">
         <v>114</v>
       </c>
@@ -16529,9 +16361,6 @@
       <c r="G109" t="s">
         <v>1187</v>
       </c>
-      <c r="H109" t="s">
-        <v>1589</v>
-      </c>
       <c r="I109" t="s">
         <v>122</v>
       </c>
@@ -16633,9 +16462,6 @@
       <c r="G110" t="s">
         <v>1187</v>
       </c>
-      <c r="H110" t="s">
-        <v>1589</v>
-      </c>
       <c r="I110" t="s">
         <v>114</v>
       </c>
@@ -16737,9 +16563,6 @@
       <c r="G111" t="s">
         <v>1187</v>
       </c>
-      <c r="H111" t="s">
-        <v>1589</v>
-      </c>
       <c r="I111" t="s">
         <v>122</v>
       </c>
@@ -20451,9 +20274,6 @@
       <c r="G147" t="s">
         <v>1186</v>
       </c>
-      <c r="H147" t="s">
-        <v>1589</v>
-      </c>
       <c r="I147" t="s">
         <v>114</v>
       </c>
@@ -20555,9 +20375,6 @@
       <c r="G148" t="s">
         <v>1186</v>
       </c>
-      <c r="H148" t="s">
-        <v>1589</v>
-      </c>
       <c r="I148" t="s">
         <v>114</v>
       </c>
@@ -20659,9 +20476,6 @@
       <c r="G149" t="s">
         <v>1186</v>
       </c>
-      <c r="H149" t="s">
-        <v>1589</v>
-      </c>
       <c r="I149" t="s">
         <v>122</v>
       </c>
@@ -20762,9 +20576,6 @@
       </c>
       <c r="G150" t="s">
         <v>1186</v>
-      </c>
-      <c r="H150" t="s">
-        <v>1589</v>
       </c>
       <c r="I150" t="s">
         <v>94</v>

</xml_diff>